<commit_message>
Implementación de la lógica de la tómbola con análisis estadístico y animación de bolas. Se añadieron funciones para predecir números basados en datos de Excel, analizar números calientes y fríos, y generar estadísticas gráficas. Se creó una interfaz gráfica con Tkinter para interactuar con la tómbola y visualizar resultados. Se implementó la animación de bolas erráticas en la interfaz.
</commit_message>
<xml_diff>
--- a/tombola-de-bolos/data/numeros_generados.xlsx
+++ b/tombola-de-bolos/data/numeros_generados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Resultados" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resultados" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2510,6 +2510,58 @@
         <v>4</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2</v>
+      </c>
+      <c r="B80" t="n">
+        <v>15</v>
+      </c>
+      <c r="C80" t="n">
+        <v>20</v>
+      </c>
+      <c r="D80" t="n">
+        <v>26</v>
+      </c>
+      <c r="E80" t="n">
+        <v>28</v>
+      </c>
+      <c r="F80" t="n">
+        <v>36</v>
+      </c>
+      <c r="G80" t="n">
+        <v>10</v>
+      </c>
+      <c r="H80" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>4</v>
+      </c>
+      <c r="B81" t="n">
+        <v>33</v>
+      </c>
+      <c r="C81" t="n">
+        <v>35</v>
+      </c>
+      <c r="D81" t="n">
+        <v>37</v>
+      </c>
+      <c r="E81" t="n">
+        <v>38</v>
+      </c>
+      <c r="F81" t="n">
+        <v>40</v>
+      </c>
+      <c r="G81" t="n">
+        <v>8</v>
+      </c>
+      <c r="H81" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>